<commit_message>
make kozu automation with compilation
</commit_message>
<xml_diff>
--- a/core/static/Расчет_анкерных_болтов.xlsx
+++ b/core/static/Расчет_анкерных_болтов.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81414815-05C2-4CB9-AB86-AB278E8181FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C44DC20-0BCD-40B3-918A-2DEE2C836513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Фланец" sheetId="4" r:id="rId1"/>
@@ -1557,26 +1557,26 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="16" max="16" width="3.33203125" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.44140625" customWidth="1"/>
-    <col min="25" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.88671875" customWidth="1"/>
-    <col min="28" max="28" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="60.44140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28.44140625" customWidth="1"/>
-    <col min="35" max="35" width="67.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" customWidth="1"/>
+    <col min="25" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.42578125" customWidth="1"/>
+    <col min="35" max="35" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="R1" s="64"/>
       <c r="S1" s="65"/>
       <c r="T1" s="65"/>
@@ -1597,7 +1597,7 @@
       <c r="AI1" s="65"/>
       <c r="AJ1" s="66"/>
     </row>
-    <row r="2" spans="1:37" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H2" s="10" t="s">
         <v>12</v>
       </c>
@@ -1657,20 +1657,20 @@
       </c>
       <c r="AJ2" s="70"/>
     </row>
-    <row r="3" spans="1:37" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:37" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="47" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I3" s="11">
         <f ca="1">OFFSET(K2,H4,2)</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J3" s="12">
         <f ca="1">OFFSET(K2,H4,3)</f>
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>17</v>
@@ -1729,20 +1729,20 @@
       </c>
       <c r="AH3" s="5" t="str">
         <f>RIGHT(H3,2)</f>
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AI3" s="5" t="s">
         <v>63</v>
       </c>
       <c r="AJ3" s="70"/>
     </row>
-    <row r="4" spans="1:37" ht="28.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:37" ht="30" x14ac:dyDescent="0.4">
       <c r="A4" s="46">
-        <v>1700</v>
+        <v>1670</v>
       </c>
       <c r="H4">
         <f>MATCH(H3,K3:K10,0)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>8</v>
@@ -1795,14 +1795,14 @@
       </c>
       <c r="AH4" s="5">
         <f>30*AH3</f>
-        <v>1440</v>
+        <v>1260</v>
       </c>
       <c r="AI4" s="6" t="s">
         <v>65</v>
       </c>
       <c r="AJ4" s="70"/>
     </row>
-    <row r="5" spans="1:37" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1856,10 +1856,10 @@
       </c>
       <c r="AJ5" s="70"/>
     </row>
-    <row r="6" spans="1:37" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="43">
         <f>A4*TAN(3.14159/12)</f>
-        <v>455.51322421749518</v>
+        <v>447.47475555483351</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>4</v>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="AJ6" s="70"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1944,10 +1944,10 @@
       <c r="AE7" s="67"/>
       <c r="AJ7" s="70"/>
     </row>
-    <row r="8" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="43">
         <f>A6/SIN(3.14159/12)</f>
-        <v>1759.9694024150015</v>
+        <v>1728.911118842972</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>9</v>
@@ -1990,7 +1990,7 @@
       <c r="AI8" s="72"/>
       <c r="AJ8" s="73"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="K9" s="5" t="s">
         <v>10</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="Z9" s="58"/>
       <c r="AD9" s="70"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2047,10 +2047,10 @@
       <c r="Z10" s="58"/>
       <c r="AD10" s="70"/>
     </row>
-    <row r="11" spans="1:37" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:37" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="48">
         <f ca="1">AH26</f>
-        <v>1899.9694024150015</v>
+        <v>1848.911118842972</v>
       </c>
       <c r="B11" s="44"/>
       <c r="K11" s="9"/>
@@ -2063,7 +2063,7 @@
       <c r="Z11" s="101"/>
       <c r="AD11" s="70"/>
     </row>
-    <row r="12" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
@@ -2086,7 +2086,7 @@
       <c r="AJ12" s="65"/>
       <c r="AK12" s="66"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2099,10 +2099,10 @@
       </c>
       <c r="AK13" s="70"/>
     </row>
-    <row r="14" spans="1:37" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:37" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="48">
         <f ca="1">A11+1.5*J3*2</f>
-        <v>2055.9694024150012</v>
+        <v>1983.911118842972</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="AK14" s="70"/>
     </row>
-    <row r="15" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -2148,7 +2148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F16" s="42" t="s">
         <v>12</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:37" ht="60.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:37" ht="63" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="E17" s="53"/>
       <c r="F17" s="52" t="str">
         <f>H3</f>
-        <v>М48</v>
+        <v>М42</v>
       </c>
       <c r="R17" s="67"/>
       <c r="S17" s="5" t="s">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="AK17" s="90"/>
     </row>
-    <row r="18" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="45">
-        <v>5434.05</v>
+        <v>3612.88</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>25</v>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="AA18" s="96">
         <f>INDEX(AB18:AB25,MATCH(F17,S18:S25,0))</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AB18" s="84">
         <v>20</v>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="AH18" s="5">
         <f>AH3*35</f>
-        <v>1680</v>
+        <v>1470</v>
       </c>
       <c r="AI18" s="86"/>
       <c r="AJ18" s="9" t="s">
@@ -2304,7 +2304,7 @@
       </c>
       <c r="AK18" s="70"/>
     </row>
-    <row r="19" spans="2:37" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:37" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
@@ -2315,23 +2315,23 @@
         <v>1</v>
       </c>
       <c r="E19" s="45">
-        <v>213.87</v>
+        <v>185.82</v>
       </c>
       <c r="H19" s="49">
         <v>1</v>
       </c>
       <c r="I19" s="15">
         <f ca="1">IF(H19=0,0,$E$22*SIN((H19-0.999)*2*PI()/$E$25))</f>
-        <v>1.6580360795467674E-4</v>
+        <v>1.6134793218355376E-4</v>
       </c>
       <c r="J19" s="16">
         <f ca="1">I19*I19</f>
-        <v>2.7490836410788144E-8</v>
+        <v>2.6033155219908664E-8</v>
       </c>
       <c r="K19" s="17"/>
       <c r="L19" s="18">
         <f t="shared" ref="L19:L54" ca="1" si="0">$E$18*I19/$J$55</f>
-        <v>5.546408826691545E-2</v>
+        <v>3.7894166409605495E-2</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="AH19" s="88">
         <f ca="1">INT(AH17*AH3/SIN(360/2/E23*3.14159/180))+1</f>
-        <v>2203</v>
+        <v>1928</v>
       </c>
       <c r="AI19" s="86"/>
       <c r="AJ19" s="9" t="s">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="AK19" s="70"/>
     </row>
-    <row r="20" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="E20" s="19">
         <f>E18/E19</f>
-        <v>25.408191892271006</v>
+        <v>19.44290173285976</v>
       </c>
       <c r="H20" s="49">
         <f>IF(H19=$E$25,0,IF(H19=0,0,H19+1))</f>
@@ -2390,16 +2390,16 @@
       </c>
       <c r="I20" s="15">
         <f t="shared" ref="I20:I54" ca="1" si="2">IF(H20=0,0,$E$22*SIN((H20-1)*2*PI()/$E$25))</f>
-        <v>0.16496311217614582</v>
+        <v>0.16053002322760365</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" ref="J20:J54" ca="1" si="3">I20*I20</f>
-        <v>2.7212828378839669E-2</v>
+        <v>2.576988835745497E-2</v>
       </c>
       <c r="K20" s="17"/>
       <c r="L20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>55.182928329423902</v>
+        <v>37.702072357545248</v>
       </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
@@ -2427,7 +2427,7 @@
       <c r="AF20" s="67"/>
       <c r="AK20" s="70"/>
     </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="E21" s="14">
         <f ca="1">A11/1000</f>
-        <v>1.8999694024150016</v>
+        <v>1.8489111188429719</v>
       </c>
       <c r="H21" s="49">
         <f t="shared" ref="H21:H54" si="4">IF(H20=$E$25,0,IF(H20=0,0,H20+1))</f>
@@ -2447,16 +2447,16 @@
       </c>
       <c r="I21" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.32491390366418199</v>
+        <v>0.31618242293154786</v>
       </c>
       <c r="J21" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10556904479429734</v>
+        <v>9.9971324570864203E-2</v>
       </c>
       <c r="K21" s="17"/>
       <c r="L21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>108.68915130546736</v>
+        <v>74.258586324675647</v>
       </c>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
@@ -2485,7 +2485,7 @@
       <c r="AG21" s="93"/>
       <c r="AK21" s="70"/>
     </row>
-    <row r="22" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="20">
         <f ca="1">E21/2</f>
-        <v>0.94998470120750078</v>
+        <v>0.92445555942148594</v>
       </c>
       <c r="H22" s="49">
         <f t="shared" si="4"/>
@@ -2503,16 +2503,16 @@
       </c>
       <c r="I22" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47499235060375034</v>
+        <v>0.46222777971074291</v>
       </c>
       <c r="J22" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22561773313207609</v>
+        <v>0.21365452033632307</v>
       </c>
       <c r="K22" s="17"/>
       <c r="L22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>158.89290941845852</v>
+        <v>108.55879072298856</v>
       </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
@@ -2540,7 +2540,7 @@
       <c r="AF22" s="67"/>
       <c r="AK22" s="70"/>
     </row>
-    <row r="23" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
@@ -2555,16 +2555,16 @@
       </c>
       <c r="I23" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.61063839532795061</v>
+        <v>0.59422857930196937</v>
       </c>
       <c r="J23" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37287924984869447</v>
+        <v>0.35310760445923689</v>
       </c>
       <c r="K23" s="17"/>
       <c r="L23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>204.26878688246151</v>
+        <v>139.56049119858213</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="AK23" s="70"/>
     </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:37" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="50"/>
@@ -2614,16 +2614,16 @@
       </c>
       <c r="I24" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.72773050140804862</v>
+        <v>0.70817404420527552</v>
       </c>
       <c r="J24" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52959168267960988</v>
+        <v>0.50151047688605555</v>
       </c>
       <c r="K24" s="17"/>
       <c r="L24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>243.43806062203453</v>
+        <v>166.32171677012295</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -2654,14 +2654,14 @@
       </c>
       <c r="AH24" s="88">
         <f ca="1">A8+I3*2</f>
-        <v>1899.9694024150015</v>
+        <v>1848.911118842972</v>
       </c>
       <c r="AI24" s="86" t="s">
         <v>88</v>
       </c>
       <c r="AK24" s="70"/>
     </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:37" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="50">
@@ -2674,16 +2674,16 @@
       </c>
       <c r="I25" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.82271088445226515</v>
+        <v>0.8006019991287614</v>
       </c>
       <c r="J25" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67685319939622834</v>
+        <v>0.64096356100896923</v>
       </c>
       <c r="K25" s="17"/>
       <c r="L25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>275.21059207520955</v>
+        <v>188.02934114045308</v>
       </c>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
@@ -2714,14 +2714,14 @@
       </c>
       <c r="AH25" s="88">
         <f ca="1">AH19</f>
-        <v>2203</v>
+        <v>1928</v>
       </c>
       <c r="AI25" s="86" t="s">
         <v>89</v>
       </c>
       <c r="AK25" s="70"/>
     </row>
-    <row r="26" spans="2:37" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:37" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="51"/>
@@ -2731,16 +2731,16 @@
       </c>
       <c r="I26" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89269361358419441</v>
+        <v>0.86870406743287909</v>
       </c>
       <c r="J26" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.79690188773400705</v>
+        <v>0.75464675677442816</v>
       </c>
       <c r="K26" s="17"/>
       <c r="L26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>298.6209889514584</v>
+        <v>204.02378912766815</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
@@ -2752,14 +2752,14 @@
       </c>
       <c r="AH26" s="88">
         <f ca="1">OFFSET(AH23,AI23,0)</f>
-        <v>1899.9694024150015</v>
+        <v>1848.911118842972</v>
       </c>
       <c r="AI26" s="92" t="s">
         <v>91</v>
       </c>
       <c r="AK26" s="70"/>
     </row>
-    <row r="27" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="50"/>
@@ -2769,16 +2769,16 @@
       </c>
       <c r="I27" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93555229899213266</v>
+        <v>0.91041100223351734</v>
       </c>
       <c r="J27" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.87525810414946481</v>
+        <v>0.82884819298783752</v>
       </c>
       <c r="K27" s="17"/>
       <c r="L27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>312.9579381879289</v>
+        <v>213.81907752325782</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
@@ -2797,7 +2797,7 @@
       <c r="AJ27" s="72"/>
       <c r="AK27" s="73"/>
     </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:37" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="50"/>
@@ -2807,21 +2807,21 @@
       </c>
       <c r="I28" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.94998470120750078</v>
+        <v>0.92445555942148594</v>
       </c>
       <c r="J28" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.90247093252830457</v>
+        <v>0.85461808134529249</v>
       </c>
       <c r="K28" s="17"/>
       <c r="L28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>317.78581883691703</v>
+        <v>217.11758144597715</v>
       </c>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
     </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:37" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="50"/>
@@ -2831,21 +2831,21 @@
       </c>
       <c r="I29" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93555229899213266</v>
+        <v>0.91041100223351734</v>
       </c>
       <c r="J29" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.87525810414946481</v>
+        <v>0.82884819298783752</v>
       </c>
       <c r="K29" s="17"/>
       <c r="L29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>312.9579381879289</v>
+        <v>213.81907752325782</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
     </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:37" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="50"/>
@@ -2855,21 +2855,21 @@
       </c>
       <c r="I30" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89269361358419452</v>
+        <v>0.8687040674328792</v>
       </c>
       <c r="J30" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.79690188773400716</v>
+        <v>0.75464675677442838</v>
       </c>
       <c r="K30" s="17"/>
       <c r="L30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>298.62098895145846</v>
+        <v>204.02378912766818</v>
       </c>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
     </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:37" x14ac:dyDescent="0.25">
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="50"/>
@@ -2879,84 +2879,84 @@
       </c>
       <c r="I31" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.82271088445226526</v>
+        <v>0.80060199912876151</v>
       </c>
       <c r="J31" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67685319939622857</v>
+        <v>0.64096356100896945</v>
       </c>
       <c r="K31" s="17"/>
       <c r="L31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>275.2105920752096</v>
+        <v>188.02934114045308</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
     </row>
-    <row r="32" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:37" x14ac:dyDescent="0.25">
       <c r="H32" s="49">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="I32" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.72773050140804862</v>
+        <v>0.70817404420527552</v>
       </c>
       <c r="J32" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52959168267960988</v>
+        <v>0.50151047688605555</v>
       </c>
       <c r="K32" s="17"/>
       <c r="L32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>243.43806062203453</v>
+        <v>166.32171677012295</v>
       </c>
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H33" s="49">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="I33" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.61063839532795083</v>
+        <v>0.59422857930196959</v>
       </c>
       <c r="J33" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37287924984869475</v>
+        <v>0.35310760445923717</v>
       </c>
       <c r="K33" s="17"/>
       <c r="L33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>204.26878688246157</v>
+        <v>139.56049119858218</v>
       </c>
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H34" s="49">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I34" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.47499235060375072</v>
+        <v>0.4622277797107433</v>
       </c>
       <c r="J34" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22561773313207645</v>
+        <v>0.21365452033632343</v>
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>158.89290941845863</v>
+        <v>108.55879072298865</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="50"/>
@@ -2966,21 +2966,21 @@
       </c>
       <c r="I35" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.32491390366418216</v>
+        <v>0.31618242293154802</v>
       </c>
       <c r="J35" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10556904479429745</v>
+        <v>9.9971324570864301E-2</v>
       </c>
       <c r="K35" s="17"/>
       <c r="L35" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>108.68915130546742</v>
+        <v>74.25858632467569</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="50"/>
@@ -2990,21 +2990,21 @@
       </c>
       <c r="I36" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16496311217614576</v>
+        <v>0.1605300232276036</v>
       </c>
       <c r="J36" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2.7212828378839649E-2</v>
+        <v>2.5769888357454949E-2</v>
       </c>
       <c r="K36" s="17"/>
       <c r="L36" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>55.182928329423881</v>
+        <v>37.702072357545241</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
     </row>
-    <row r="37" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="H37" s="49">
@@ -3013,21 +3013,21 @@
       </c>
       <c r="I37" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>1.1638722888711966E-16</v>
+        <v>1.1325953002569175E-16</v>
       </c>
       <c r="J37" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3545987048022782E-32</v>
+        <v>1.282772114164057E-32</v>
       </c>
       <c r="K37" s="17"/>
       <c r="L37" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8933480493991959E-14</v>
+        <v>2.6600126944203538E-14</v>
       </c>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
     </row>
-    <row r="38" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="22" t="s">
         <v>36</v>
       </c>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="E38" s="25">
         <f ca="1">L55+E19/E23</f>
-        <v>323.72665217025036</v>
+        <v>222.27924811264381</v>
       </c>
       <c r="H38" s="49">
         <f t="shared" si="4"/>
@@ -3045,21 +3045,21 @@
       </c>
       <c r="I38" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.16496311217614554</v>
+        <v>-0.16053002322760337</v>
       </c>
       <c r="J38" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2.7212828378839576E-2</v>
+        <v>2.5769888357454879E-2</v>
       </c>
       <c r="K38" s="17"/>
       <c r="L38" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-55.18292832942381</v>
+        <v>-37.702072357545191</v>
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
     </row>
-    <row r="39" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="26" t="s">
         <v>37</v>
       </c>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="E39" s="29">
         <f ca="1">L55-E19/E23</f>
-        <v>311.8449855035837</v>
+        <v>211.95591477931049</v>
       </c>
       <c r="H39" s="49">
         <f t="shared" si="4"/>
@@ -3077,37 +3077,37 @@
       </c>
       <c r="I39" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.32491390366418194</v>
+        <v>-0.3161824229315478</v>
       </c>
       <c r="J39" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1055690447942973</v>
+        <v>9.9971324570864162E-2</v>
       </c>
       <c r="K39" s="17"/>
       <c r="L39" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-108.68915130546733</v>
+        <v>-74.258586324675647</v>
       </c>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
     </row>
-    <row r="40" spans="2:21" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:21" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H40" s="49">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="I40" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.4749923506037505</v>
+        <v>-0.46222777971074308</v>
       </c>
       <c r="J40" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22561773313207623</v>
+        <v>0.21365452033632323</v>
       </c>
       <c r="K40" s="17"/>
       <c r="L40" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-158.89290941845857</v>
+        <v>-108.55879072298859</v>
       </c>
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
@@ -3118,7 +3118,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="30" t="s">
         <v>38</v>
       </c>
@@ -3140,29 +3140,29 @@
       </c>
       <c r="I41" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.61063839532795028</v>
+        <v>-0.59422857930196904</v>
       </c>
       <c r="J41" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37287924984869408</v>
+        <v>0.3531076044592365</v>
       </c>
       <c r="K41" s="17"/>
       <c r="L41" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-204.2687868824614</v>
+        <v>-139.56049119858207</v>
       </c>
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="T41" s="79">
         <f ca="1">1.35*E38/W3*10</f>
-        <v>9.7117995651075102</v>
+        <v>6.6683774433793142</v>
       </c>
       <c r="U41" s="100">
         <f>INDEX(E43:E49,MATCH(F17,B43:B49,0))</f>
-        <v>662.4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="31" t="s">
         <v>41</v>
       </c>
@@ -3176,21 +3176,21 @@
       </c>
       <c r="I42" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.72773050140804851</v>
+        <v>-0.70817404420527541</v>
       </c>
       <c r="J42" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52959168267960965</v>
+        <v>0.50151047688605532</v>
       </c>
       <c r="K42" s="17"/>
       <c r="L42" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-243.4380606220345</v>
+        <v>-166.32171677012292</v>
       </c>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="33" t="s">
         <v>8</v>
       </c>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="D43" s="61">
         <f t="shared" ref="D43:D49" ca="1" si="5">$E$38/C43</f>
-        <v>2.0379392645278589</v>
+        <v>1.3993027895035808</v>
       </c>
       <c r="E43" s="34">
         <f>$W$3*T4/10</f>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="F43" s="63">
         <f ca="1">$E$39/E43</f>
-        <v>1.9631412370386132</v>
+        <v>1.3343148553938338</v>
       </c>
       <c r="H43" s="49">
         <f t="shared" si="4"/>
@@ -3216,21 +3216,21 @@
       </c>
       <c r="I43" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.82271088445226492</v>
+        <v>-0.80060199912876118</v>
       </c>
       <c r="J43" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67685319939622801</v>
+        <v>0.6409635610089689</v>
       </c>
       <c r="K43" s="17"/>
       <c r="L43" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-275.21059207520949</v>
+        <v>-188.02934114045303</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44" s="33" t="s">
         <v>6</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="D44" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2820857511693085</v>
+        <v>0.88031385391146066</v>
       </c>
       <c r="E44" s="34">
         <f>$W$3*T5/10</f>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="F44" s="63">
         <f t="shared" ref="F44:F49" ca="1" si="6">$E$39/E44</f>
-        <v>1.2352742543219795</v>
+        <v>0.83959562202143201</v>
       </c>
       <c r="H44" s="49">
         <f t="shared" si="4"/>
@@ -3255,21 +3255,21 @@
       </c>
       <c r="I44" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.89269361358419452</v>
+        <v>-0.8687040674328792</v>
       </c>
       <c r="J44" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.79690188773400716</v>
+        <v>0.75464675677442838</v>
       </c>
       <c r="K44" s="17"/>
       <c r="L44" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-298.62098895145846</v>
+        <v>-204.02378912766818</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="33" t="s">
         <v>4</v>
       </c>
@@ -3278,7 +3278,7 @@
       </c>
       <c r="D45" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.8816085298754095</v>
+        <v>0.60533564300828924</v>
       </c>
       <c r="E45" s="34">
         <f t="shared" ref="E45:E49" si="7">$W$3*T6/10</f>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="F45" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.84925104984636091</v>
+        <v>0.57722199013973452</v>
       </c>
       <c r="H45" s="49">
         <f t="shared" si="4"/>
@@ -3294,21 +3294,21 @@
       </c>
       <c r="I45" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.93555229899213266</v>
+        <v>-0.91041100223351734</v>
       </c>
       <c r="J45" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.87525810414946481</v>
+        <v>0.82884819298783752</v>
       </c>
       <c r="K45" s="17"/>
       <c r="L45" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-312.9579381879289</v>
+        <v>-213.81907752325782</v>
       </c>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="33" t="s">
         <v>5</v>
       </c>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="D46" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.64231478605208403</v>
+        <v>0.44103025419175362</v>
       </c>
       <c r="E46" s="34">
         <f t="shared" si="7"/>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="F46" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.6187400506023486</v>
+        <v>0.42054744995894938</v>
       </c>
       <c r="H46" s="49">
         <f t="shared" si="4"/>
@@ -3333,21 +3333,21 @@
       </c>
       <c r="I46" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.94998470120750078</v>
+        <v>-0.92445555942148594</v>
       </c>
       <c r="J46" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.90247093252830457</v>
+        <v>0.85461808134529249</v>
       </c>
       <c r="K46" s="17"/>
       <c r="L46" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-317.78581883691703</v>
+        <v>-217.11758144597715</v>
       </c>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="33" t="s">
         <v>9</v>
       </c>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="D47" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48871777199615091</v>
+        <v>0.33556649775459513</v>
       </c>
       <c r="E47" s="34">
         <f t="shared" si="7"/>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="F47" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.47078047328439571</v>
+        <v>0.31998175540354845</v>
       </c>
       <c r="H47" s="49">
         <f t="shared" si="4"/>
@@ -3373,21 +3373,21 @@
       </c>
       <c r="I47" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.93555229899213277</v>
+        <v>-0.91041100223351745</v>
       </c>
       <c r="J47" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.87525810414946503</v>
+        <v>0.82884819298783774</v>
       </c>
       <c r="K47" s="17"/>
       <c r="L47" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-312.9579381879289</v>
+        <v>-213.81907752325785</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="33" t="s">
         <v>10</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="D48" s="61">
         <f t="shared" ca="1" si="5"/>
-        <v>0.40921078519814236</v>
+        <v>0.28097490596971791</v>
       </c>
       <c r="E48" s="34">
         <f t="shared" si="7"/>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="F48" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.39419161358056343</v>
+        <v>0.26792556538909179</v>
       </c>
       <c r="H48" s="49">
         <f t="shared" si="4"/>
@@ -3413,21 +3413,21 @@
       </c>
       <c r="I48" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.89269361358419441</v>
+        <v>-0.86870406743287909</v>
       </c>
       <c r="J48" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.79690188773400705</v>
+        <v>0.75464675677442816</v>
       </c>
       <c r="K48" s="17"/>
       <c r="L48" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-298.6209889514584</v>
+        <v>-204.02378912766815</v>
       </c>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
     </row>
-    <row r="49" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="35" t="s">
         <v>11</v>
       </c>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="D49" s="62">
         <f t="shared" ca="1" si="5"/>
-        <v>0.35438057161494291</v>
+        <v>0.24332703679545026</v>
       </c>
       <c r="E49" s="34">
         <f t="shared" si="7"/>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="F49" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>0.34137382102198544</v>
+        <v>0.2320261792876962</v>
       </c>
       <c r="H49" s="49">
         <f t="shared" si="4"/>
@@ -3453,42 +3453,42 @@
       </c>
       <c r="I49" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.82271088445226559</v>
+        <v>-0.80060199912876184</v>
       </c>
       <c r="J49" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67685319939622912</v>
+        <v>0.64096356100897001</v>
       </c>
       <c r="K49" s="17"/>
       <c r="L49" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-275.21059207520972</v>
+        <v>-188.02934114045317</v>
       </c>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
     </row>
-    <row r="50" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H50" s="49">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="I50" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.72773050140804874</v>
+        <v>-0.70817404420527563</v>
       </c>
       <c r="J50" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52959168267960999</v>
+        <v>0.50151047688605566</v>
       </c>
       <c r="K50" s="17"/>
       <c r="L50" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-243.43806062203458</v>
+        <v>-166.32171677012295</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
     </row>
-    <row r="51" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="104" t="s">
         <v>50</v>
       </c>
@@ -3503,90 +3503,90 @@
       </c>
       <c r="I51" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.61063839532795094</v>
+        <v>-0.59422857930196971</v>
       </c>
       <c r="J51" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37287924984869492</v>
+        <v>0.35310760445923728</v>
       </c>
       <c r="K51" s="17"/>
       <c r="L51" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-204.26878688246163</v>
+        <v>-139.56049119858224</v>
       </c>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H52" s="49">
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="I52" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.47499235060375006</v>
+        <v>-0.46222777971074264</v>
       </c>
       <c r="J52" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22561773313207581</v>
+        <v>0.21365452033632282</v>
       </c>
       <c r="K52" s="17"/>
       <c r="L52" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-158.8929094184584</v>
+        <v>-108.55879072298849</v>
       </c>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H53" s="49">
         <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="I53" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.32491390366418188</v>
+        <v>-0.31618242293154775</v>
       </c>
       <c r="J53" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.10556904479429727</v>
+        <v>9.9971324570864134E-2</v>
       </c>
       <c r="K53" s="17"/>
       <c r="L53" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-108.68915130546732</v>
+        <v>-74.258586324675633</v>
       </c>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
     </row>
-    <row r="54" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H54" s="49">
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="I54" s="15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.16496311217614587</v>
+        <v>-0.16053002322760371</v>
       </c>
       <c r="J54" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>2.7212828378839687E-2</v>
+        <v>2.5769888357454987E-2</v>
       </c>
       <c r="K54" s="37"/>
       <c r="L54" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>-55.182928329423923</v>
+        <v>-37.702072357545262</v>
       </c>
       <c r="M54" s="37"/>
       <c r="N54" s="37"/>
     </row>
-    <row r="55" spans="2:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="75" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="77">
         <f ca="1">A11</f>
-        <v>1899.9694024150015</v>
+        <v>1848.911118842972</v>
       </c>
       <c r="H55" s="38">
         <f>MAX(H19:H54)</f>
@@ -3595,12 +3595,12 @@
       <c r="I55" s="28"/>
       <c r="J55" s="39">
         <f ca="1">SUM(J19:J54)</f>
-        <v>16.244476813000322</v>
+        <v>15.383125490248419</v>
       </c>
       <c r="K55" s="28"/>
       <c r="L55" s="40">
         <f ca="1">MAX(L19:L54)</f>
-        <v>317.78581883691703</v>
+        <v>217.11758144597715</v>
       </c>
       <c r="M55" s="40">
         <f>SUM(M19:M54)</f>
@@ -3611,14 +3611,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="2:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="2:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="75" t="s">
         <v>69</v>
       </c>
       <c r="C57" s="76">
         <f>AH4*AH5*AH6</f>
-        <v>1440</v>
+        <v>1260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>